<commit_message>
Add Tests for u-3 instructions ( CLA, MQL, MQA, SWP, CAM ).
Tests are the same as for IOs, only increment PC.
</commit_message>
<xml_diff>
--- a/Docs/Testing Plan.xlsx
+++ b/Docs/Testing Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="203">
   <si>
     <t>PDP-8 Instruction List</t>
   </si>
@@ -590,6 +590,39 @@
   </si>
   <si>
     <t>Check 12th bit for sign and skip next instruction if it is 1 ( neg ). Ie increment PC</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>Will Add test cases I made while coding into this documentation</t>
+  </si>
+  <si>
+    <t>Increment PC</t>
+  </si>
+  <si>
+    <t>Microinstruction 3</t>
+  </si>
+  <si>
+    <t>Note: These instructions are treated as NOP, just increment PC and move on.</t>
+  </si>
+  <si>
+    <t>M3_CLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MQL </t>
+  </si>
+  <si>
+    <t>MQA</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>All IO ( increment PC )</t>
+  </si>
+  <si>
+    <t>SWP</t>
   </si>
 </sst>
 </file>
@@ -649,7 +682,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +710,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -829,6 +868,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1133,191 +1185,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF55"/>
+  <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.5703125" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B1" s="33"/>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>71</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>71</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>71</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>71</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4">
+      <c r="B4" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4">
         <v>7777</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>5252</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2525</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -1347,166 +1432,169 @@
       <c r="AD11" s="23"/>
       <c r="AE11" s="23"/>
       <c r="AF11" s="23"/>
-    </row>
-    <row r="12" spans="1:32" ht="60" x14ac:dyDescent="0.25">
+      <c r="AG11" s="23"/>
+    </row>
+    <row r="12" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="D12" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="E12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="H12" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="24"/>
+      <c r="J12" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="K12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="24"/>
+      <c r="M12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="N12" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="24"/>
+      <c r="P12" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="Q12" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24" t="s">
+      <c r="R12" s="24"/>
+      <c r="S12" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="S12" s="24" t="s">
+      <c r="T12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24" t="s">
+      <c r="U12" s="24"/>
+      <c r="V12" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="V12" s="24" t="s">
+      <c r="W12" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24" t="s">
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Y12" s="24" t="s">
+      <c r="Z12" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24" t="s">
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AB12" s="24" t="s">
+      <c r="AC12" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="24" t="s">
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AE12" s="24" t="s">
+      <c r="AF12" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AF12" s="24"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG12" s="24"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="H13" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="21"/>
+      <c r="J13" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="K13" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21" t="s">
+      <c r="L13" s="21"/>
+      <c r="M13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="N13" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="21"/>
+      <c r="P13" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="Q13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21" t="s">
+      <c r="R13" s="21"/>
+      <c r="S13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="T13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21" t="s">
+      <c r="U13" s="21"/>
+      <c r="V13" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="V13" s="21" t="s">
+      <c r="W13" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21" t="s">
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="Y13" s="21" t="s">
+      <c r="Z13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21" t="s">
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AB13" s="21" t="s">
+      <c r="AC13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21" t="s">
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE13" s="21" t="s">
+      <c r="AF13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF13" s="21"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG13" s="21"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
-      <c r="B14" s="9"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -1537,35 +1625,38 @@
       <c r="AD14" s="9"/>
       <c r="AE14" s="9"/>
       <c r="AF14" s="9"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG14" s="9"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="10">
+      <c r="D15" s="10">
         <v>7777</v>
       </c>
-      <c r="D15" s="10">
+      <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10">
         <v>1111</v>
       </c>
-      <c r="G15" s="10">
+      <c r="H15" s="10">
         <v>0</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10">
-        <v>0</v>
-      </c>
+      <c r="I15" s="10"/>
       <c r="J15" s="10">
         <v>0</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1587,11 +1678,12 @@
       <c r="AD15" s="10"/>
       <c r="AE15" s="10"/>
       <c r="AF15" s="10"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG15" s="10"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1621,208 +1713,215 @@
       <c r="AD16" s="10"/>
       <c r="AE16" s="10"/>
       <c r="AF16" s="10"/>
-    </row>
-    <row r="17" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG16" s="10"/>
+    </row>
+    <row r="17" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="K17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9" t="s">
+      <c r="O17" s="9"/>
+      <c r="P17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="Q17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9" t="s">
+      <c r="R17" s="9"/>
+      <c r="S17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="S17" s="9" t="s">
+      <c r="T17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9" t="s">
+      <c r="U17" s="9"/>
+      <c r="V17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="V17" s="9" t="s">
+      <c r="W17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9" t="s">
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="Y17" s="9" t="s">
+      <c r="Z17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9" t="s">
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AB17" s="9" t="s">
+      <c r="AC17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9" t="s">
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AE17" s="9" t="s">
+      <c r="AF17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AF17" s="9"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG17" s="9"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="12"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="K18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="9"/>
+      <c r="M18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="M18" s="9" t="s">
+      <c r="N18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9" t="s">
+      <c r="O18" s="9"/>
+      <c r="P18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="Q18" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9" t="s">
+      <c r="R18" s="9"/>
+      <c r="S18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="S18" s="9" t="s">
+      <c r="T18" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9" t="s">
+      <c r="U18" s="9"/>
+      <c r="V18" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V18" s="9" t="s">
+      <c r="W18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9" t="s">
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Y18" s="9" t="s">
+      <c r="Z18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9" t="s">
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AB18" s="9" t="s">
+      <c r="AC18" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9" t="s">
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AE18" s="9" t="s">
+      <c r="AF18" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AF18" s="9"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG18" s="9"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="H19" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="10"/>
+      <c r="J19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="K19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="N19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10" t="s">
+      <c r="O19" s="10"/>
+      <c r="P19" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="Q19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10" t="s">
+      <c r="R19" s="10"/>
+      <c r="S19" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="T19" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="T19" s="10"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -1835,11 +1934,12 @@
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
       <c r="AF19" s="10"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG19" s="10"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1869,28 +1969,31 @@
       <c r="AD20" s="10"/>
       <c r="AE20" s="10"/>
       <c r="AF20" s="10"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG20" s="10"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -1915,11 +2018,12 @@
       <c r="AD21" s="11"/>
       <c r="AE21" s="11"/>
       <c r="AF21" s="11"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG21" s="11"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -1949,770 +2053,787 @@
       <c r="AD22" s="11"/>
       <c r="AE22" s="11"/>
       <c r="AF22" s="11"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG22" s="11"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="10"/>
+      <c r="J23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="K23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10" t="s">
+      <c r="L23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="N23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10" t="s">
+      <c r="O23" s="10"/>
+      <c r="P23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="Q23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10" t="s">
+      <c r="R23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="S23" s="10" t="s">
+      <c r="T23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10" t="s">
+      <c r="U23" s="10"/>
+      <c r="V23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="V23" s="10" t="s">
+      <c r="W23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10" t="s">
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="Y23" s="10" t="s">
+      <c r="Z23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10" t="s">
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="AB23" s="10" t="s">
+      <c r="AC23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10" t="s">
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="AE23" s="10" t="s">
+      <c r="AF23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="AF23" s="10"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG23" s="10"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="H24" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="10"/>
+      <c r="J24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="K24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10" t="s">
+      <c r="L24" s="10"/>
+      <c r="M24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M24" s="10" t="s">
+      <c r="N24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10" t="s">
+      <c r="O24" s="10"/>
+      <c r="P24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="P24" s="10" t="s">
+      <c r="Q24" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10" t="s">
+      <c r="R24" s="10"/>
+      <c r="S24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="S24" s="10" t="s">
+      <c r="T24" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="10"/>
+      <c r="V24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="V24" s="10" t="s">
+      <c r="W24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10" t="s">
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="Y24" s="10" t="s">
+      <c r="Z24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="10" t="s">
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AB24" s="10" t="s">
+      <c r="AC24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="AC24" s="10"/>
-      <c r="AD24" s="10" t="s">
+      <c r="AD24" s="10"/>
+      <c r="AE24" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AE24" s="10" t="s">
+      <c r="AF24" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="AF24" s="10"/>
-    </row>
-    <row r="25" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG24" s="10"/>
+    </row>
+    <row r="25" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="H25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="11"/>
+      <c r="J25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="K25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11" t="s">
+      <c r="L25" s="11"/>
+      <c r="M25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M25" s="9" t="s">
+      <c r="N25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11" t="s">
+      <c r="O25" s="11"/>
+      <c r="P25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="P25" s="9" t="s">
+      <c r="Q25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11" t="s">
+      <c r="R25" s="11"/>
+      <c r="S25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="T25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11" t="s">
+      <c r="U25" s="11"/>
+      <c r="V25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="V25" s="9" t="s">
+      <c r="W25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11" t="s">
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="Y25" s="9" t="s">
+      <c r="Z25" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11" t="s">
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="AB25" s="9" t="s">
+      <c r="AC25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AC25" s="11"/>
-      <c r="AD25" s="11" t="s">
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="AE25" s="9" t="s">
+      <c r="AF25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AF25" s="11"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG25" s="11"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="11" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="H26" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="11"/>
+      <c r="J26" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11" t="s">
+      <c r="L26" s="11"/>
+      <c r="M26" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="N26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11" t="s">
+      <c r="O26" s="11"/>
+      <c r="P26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P26" s="11" t="s">
+      <c r="Q26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11" t="s">
+      <c r="R26" s="11"/>
+      <c r="S26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="S26" s="11" t="s">
+      <c r="T26" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11" t="s">
+      <c r="U26" s="11"/>
+      <c r="V26" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="V26" s="11" t="s">
+      <c r="W26" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11" t="s">
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Y26" s="11" t="s">
+      <c r="Z26" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11" t="s">
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AB26" s="11" t="s">
+      <c r="AC26" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AC26" s="11"/>
-      <c r="AD26" s="11" t="s">
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AE26" s="11" t="s">
+      <c r="AF26" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AF26" s="11"/>
-    </row>
-    <row r="27" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG26" s="11"/>
+    </row>
+    <row r="27" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="H27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="10"/>
+      <c r="J27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="K27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10" t="s">
+      <c r="L27" s="10"/>
+      <c r="M27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="N27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10" t="s">
+      <c r="O27" s="10"/>
+      <c r="P27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P27" s="10" t="s">
+      <c r="Q27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10" t="s">
+      <c r="R27" s="10"/>
+      <c r="S27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="S27" s="10" t="s">
+      <c r="T27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="10"/>
+      <c r="V27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="V27" s="10" t="s">
+      <c r="W27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10" t="s">
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="Y27" s="10" t="s">
+      <c r="Z27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="Z27" s="10"/>
-      <c r="AA27" s="10" t="s">
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="AB27" s="10" t="s">
+      <c r="AC27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AC27" s="10"/>
-      <c r="AD27" s="10" t="s">
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="AE27" s="10" t="s">
+      <c r="AF27" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AF27" s="10"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG27" s="10"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="H28" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="10"/>
+      <c r="J28" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J28" s="10" t="s">
+      <c r="K28" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M28" s="10" t="s">
+      <c r="N28" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10" t="s">
+      <c r="O28" s="10"/>
+      <c r="P28" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="P28" s="10" t="s">
+      <c r="Q28" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10" t="s">
+      <c r="R28" s="10"/>
+      <c r="S28" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="S28" s="10" t="s">
+      <c r="T28" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10" t="s">
+      <c r="U28" s="10"/>
+      <c r="V28" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="V28" s="10" t="s">
+      <c r="W28" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="W28" s="10"/>
-      <c r="X28" s="10" t="s">
+      <c r="X28" s="10"/>
+      <c r="Y28" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Y28" s="10" t="s">
+      <c r="Z28" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="10" t="s">
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AB28" s="10" t="s">
+      <c r="AC28" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="AC28" s="10"/>
-      <c r="AD28" s="10" t="s">
+      <c r="AD28" s="10"/>
+      <c r="AE28" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AE28" s="10" t="s">
+      <c r="AF28" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AF28" s="10"/>
-    </row>
-    <row r="29" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG28" s="10"/>
+    </row>
+    <row r="29" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="11"/>
+      <c r="J29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="K29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11" t="s">
+      <c r="L29" s="11"/>
+      <c r="M29" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M29" s="9" t="s">
+      <c r="N29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11" t="s">
+      <c r="O29" s="11"/>
+      <c r="P29" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="P29" s="9" t="s">
+      <c r="Q29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11" t="s">
+      <c r="R29" s="11"/>
+      <c r="S29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="S29" s="9" t="s">
+      <c r="T29" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="11"/>
-      <c r="U29" s="16" t="s">
+      <c r="U29" s="11"/>
+      <c r="V29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="V29" s="9" t="s">
+      <c r="W29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="W29" s="11"/>
-      <c r="X29" s="16" t="s">
+      <c r="X29" s="11"/>
+      <c r="Y29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="Y29" s="9" t="s">
+      <c r="Z29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="16" t="s">
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="AB29" s="9" t="s">
+      <c r="AC29" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="15" t="s">
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AE29" s="9" t="s">
+      <c r="AF29" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AF29" s="11"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG29" s="11"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="H30" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11" t="s">
+      <c r="I30" s="11"/>
+      <c r="J30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="J30" s="11" t="s">
+      <c r="K30" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11" t="s">
+      <c r="L30" s="11"/>
+      <c r="M30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="M30" s="11" t="s">
+      <c r="N30" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11" t="s">
+      <c r="O30" s="11"/>
+      <c r="P30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="11" t="s">
+      <c r="Q30" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11" t="s">
+      <c r="R30" s="11"/>
+      <c r="S30" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="S30" s="11" t="s">
+      <c r="T30" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11" t="s">
+      <c r="U30" s="11"/>
+      <c r="V30" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="V30" s="11" t="s">
+      <c r="W30" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11" t="s">
+      <c r="X30" s="11"/>
+      <c r="Y30" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Y30" s="11" t="s">
+      <c r="Z30" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11" t="s">
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AB30" s="11" t="s">
+      <c r="AC30" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="11" t="s">
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AE30" s="11" t="s">
+      <c r="AF30" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="AF30" s="11"/>
-    </row>
-    <row r="31" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG30" s="11"/>
+    </row>
+    <row r="31" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="10"/>
+      <c r="J31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="K31" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10" t="s">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="M31" s="10" t="s">
+      <c r="N31" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10" t="s">
+      <c r="O31" s="10"/>
+      <c r="P31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P31" s="10" t="s">
+      <c r="Q31" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10" t="s">
+      <c r="R31" s="10"/>
+      <c r="S31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="S31" s="10" t="s">
+      <c r="T31" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10" t="s">
+      <c r="U31" s="10"/>
+      <c r="V31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="V31" s="10" t="s">
+      <c r="W31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="W31" s="10"/>
-      <c r="X31" s="10" t="s">
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="Y31" s="10" t="s">
+      <c r="Z31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="Z31" s="10"/>
-      <c r="AA31" s="10" t="s">
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="AB31" s="10" t="s">
+      <c r="AC31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AC31" s="10"/>
-      <c r="AD31" s="10" t="s">
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="AE31" s="10" t="s">
+      <c r="AF31" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AF31" s="10"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG31" s="10"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="10"/>
+      <c r="J32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10" t="s">
+      <c r="L32" s="10"/>
+      <c r="M32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M32" s="10" t="s">
+      <c r="N32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10" t="s">
+      <c r="O32" s="10"/>
+      <c r="P32" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="10" t="s">
+      <c r="Q32" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10" t="s">
+      <c r="R32" s="10"/>
+      <c r="S32" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="S32" s="10" t="s">
+      <c r="T32" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="T32" s="10"/>
-      <c r="U32" s="10" t="s">
+      <c r="U32" s="10"/>
+      <c r="V32" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="V32" s="10" t="s">
+      <c r="W32" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="W32" s="10"/>
-      <c r="X32" s="10" t="s">
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Y32" s="10" t="s">
+      <c r="Z32" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="Z32" s="10"/>
-      <c r="AA32" s="10" t="s">
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AB32" s="10" t="s">
+      <c r="AC32" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="AC32" s="10"/>
-      <c r="AD32" s="10" t="s">
+      <c r="AD32" s="10"/>
+      <c r="AE32" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AE32" s="10" t="s">
+      <c r="AF32" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="AF32" s="10"/>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG32" s="10"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
-      <c r="B33" s="17"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -2743,10 +2864,11 @@
       <c r="AD33" s="17"/>
       <c r="AE33" s="17"/>
       <c r="AF33" s="17"/>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG33" s="17"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
-      <c r="B34" s="17"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -2777,12 +2899,13 @@
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
       <c r="AF34" s="17"/>
-    </row>
-    <row r="35" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AG34" s="17"/>
+    </row>
+    <row r="35" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
@@ -2813,910 +2936,936 @@
       <c r="AD35" s="26"/>
       <c r="AE35" s="26"/>
       <c r="AF35" s="26"/>
-    </row>
-    <row r="36" spans="1:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AG35" s="26"/>
+    </row>
+    <row r="36" spans="1:33" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25"/>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="D36" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="E36" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="24"/>
+      <c r="G36" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="H36" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24" t="s">
+      <c r="I36" s="24"/>
+      <c r="J36" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="K36" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24" t="s">
+      <c r="L36" s="24"/>
+      <c r="M36" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="M36" s="24" t="s">
+      <c r="N36" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24" t="s">
+      <c r="O36" s="24"/>
+      <c r="P36" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="P36" s="24" t="s">
+      <c r="Q36" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24" t="s">
+      <c r="R36" s="24"/>
+      <c r="S36" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="S36" s="24" t="s">
+      <c r="T36" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24" t="s">
+      <c r="U36" s="24"/>
+      <c r="V36" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="V36" s="24" t="s">
+      <c r="W36" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W36" s="24"/>
-      <c r="X36" s="24" t="s">
+      <c r="X36" s="24"/>
+      <c r="Y36" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Y36" s="24" t="s">
+      <c r="Z36" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="Z36" s="24"/>
-      <c r="AA36" s="24" t="s">
+      <c r="AA36" s="24"/>
+      <c r="AB36" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AB36" s="24" t="s">
+      <c r="AC36" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AC36" s="24"/>
-      <c r="AD36" s="24" t="s">
+      <c r="AD36" s="24"/>
+      <c r="AE36" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AE36" s="24" t="s">
+      <c r="AF36" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AF36" s="24"/>
-    </row>
-    <row r="37" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+      <c r="AG36" s="24"/>
+    </row>
+    <row r="37" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D37" s="11"/>
       <c r="E37" s="11"/>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="11"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="11" t="s">
+      <c r="I37" s="11"/>
+      <c r="J37" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="J37" s="11"/>
       <c r="K37" s="11"/>
-      <c r="L37" s="11" t="s">
+      <c r="L37" s="11"/>
+      <c r="M37" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="M37" s="11"/>
       <c r="N37" s="11"/>
-      <c r="O37" s="11" t="s">
+      <c r="O37" s="11"/>
+      <c r="P37" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="P37" s="11"/>
       <c r="Q37" s="11"/>
-      <c r="R37" s="11" t="s">
+      <c r="R37" s="11"/>
+      <c r="S37" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="S37" s="11"/>
       <c r="T37" s="11"/>
-      <c r="U37" s="11" t="s">
+      <c r="U37" s="11"/>
+      <c r="V37" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="V37" s="11"/>
       <c r="W37" s="11"/>
-      <c r="X37" s="11" t="s">
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="Y37" s="11"/>
       <c r="Z37" s="11"/>
-      <c r="AA37" s="16" t="s">
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="AB37" s="15"/>
       <c r="AC37" s="15"/>
-      <c r="AD37" s="16" t="s">
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="AE37" s="15"/>
-      <c r="AF37" s="11"/>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF37" s="15"/>
+      <c r="AG37" s="11"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="11" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="11"/>
+      <c r="G38" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="H38" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11" t="s">
+      <c r="I38" s="11"/>
+      <c r="J38" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="K38" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11" t="s">
+      <c r="L38" s="11"/>
+      <c r="M38" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="M38" s="11" t="s">
+      <c r="N38" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11" t="s">
+      <c r="O38" s="11"/>
+      <c r="P38" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="P38" s="11" t="s">
+      <c r="Q38" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11" t="s">
+      <c r="R38" s="11"/>
+      <c r="S38" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="S38" s="11" t="s">
+      <c r="T38" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11" t="s">
+      <c r="U38" s="11"/>
+      <c r="V38" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="V38" s="11" t="s">
+      <c r="W38" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="W38" s="11"/>
-      <c r="X38" s="11" t="s">
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="Y38" s="11" t="s">
+      <c r="Z38" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="Z38" s="11"/>
-      <c r="AA38" s="16" t="s">
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AB38" s="15" t="s">
+      <c r="AC38" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="16" t="s">
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AE38" s="15" t="s">
+      <c r="AF38" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="AF38" s="11"/>
-    </row>
-    <row r="39" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG38" s="11"/>
+    </row>
+    <row r="39" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D39" s="10"/>
       <c r="E39" s="10"/>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="G39" s="10"/>
       <c r="H39" s="10"/>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="10"/>
+      <c r="J39" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="J39" s="10"/>
       <c r="K39" s="10"/>
-      <c r="L39" s="10" t="s">
+      <c r="L39" s="10"/>
+      <c r="M39" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="M39" s="10"/>
       <c r="N39" s="10"/>
-      <c r="O39" s="10" t="s">
+      <c r="O39" s="10"/>
+      <c r="P39" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
-      <c r="R39" s="10" t="s">
+      <c r="R39" s="10"/>
+      <c r="S39" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="S39" s="10"/>
       <c r="T39" s="10"/>
-      <c r="U39" s="10" t="s">
+      <c r="U39" s="10"/>
+      <c r="V39" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="V39" s="10"/>
       <c r="W39" s="10"/>
-      <c r="X39" s="10" t="s">
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="Y39" s="10"/>
       <c r="Z39" s="10"/>
-      <c r="AA39" s="31" t="s">
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="AB39" s="32"/>
       <c r="AC39" s="32"/>
-      <c r="AD39" s="31" t="s">
+      <c r="AD39" s="32"/>
+      <c r="AE39" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="AE39" s="32"/>
-      <c r="AF39" s="10"/>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF39" s="32"/>
+      <c r="AG39" s="10"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="10" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="H40" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10" t="s">
+      <c r="I40" s="10"/>
+      <c r="J40" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="K40" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="10"/>
+      <c r="M40" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="M40" s="10" t="s">
+      <c r="N40" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10" t="s">
+      <c r="O40" s="10"/>
+      <c r="P40" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="P40" s="10" t="s">
+      <c r="Q40" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10" t="s">
+      <c r="R40" s="10"/>
+      <c r="S40" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="S40" s="10" t="s">
+      <c r="T40" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10" t="s">
+      <c r="U40" s="10"/>
+      <c r="V40" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="V40" s="10" t="s">
+      <c r="W40" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="W40" s="10"/>
-      <c r="X40" s="10" t="s">
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="Y40" s="10" t="s">
+      <c r="Z40" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="Z40" s="10"/>
-      <c r="AA40" s="31" t="s">
+      <c r="AA40" s="10"/>
+      <c r="AB40" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AB40" s="32" t="s">
+      <c r="AC40" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="AC40" s="32"/>
-      <c r="AD40" s="31" t="s">
+      <c r="AD40" s="32"/>
+      <c r="AE40" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AE40" s="32" t="s">
+      <c r="AF40" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="AF40" s="10"/>
-    </row>
-    <row r="41" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG40" s="10"/>
+    </row>
+    <row r="41" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D41" s="11"/>
       <c r="E41" s="11"/>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="11"/>
+      <c r="G41" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G41" s="11"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="11" t="s">
+      <c r="I41" s="11"/>
+      <c r="J41" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J41" s="11"/>
       <c r="K41" s="11"/>
-      <c r="L41" s="11" t="s">
+      <c r="L41" s="11"/>
+      <c r="M41" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="M41" s="11"/>
       <c r="N41" s="11"/>
-      <c r="O41" s="11" t="s">
+      <c r="O41" s="11"/>
+      <c r="P41" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="P41" s="11"/>
       <c r="Q41" s="11"/>
-      <c r="R41" s="11" t="s">
+      <c r="R41" s="11"/>
+      <c r="S41" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="S41" s="11"/>
       <c r="T41" s="11"/>
-      <c r="U41" s="11" t="s">
+      <c r="U41" s="11"/>
+      <c r="V41" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="V41" s="11"/>
       <c r="W41" s="11"/>
-      <c r="X41" s="11" t="s">
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="Y41" s="11"/>
       <c r="Z41" s="11"/>
-      <c r="AA41" s="16" t="s">
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="AB41" s="15"/>
       <c r="AC41" s="15"/>
-      <c r="AD41" s="16" t="s">
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="11"/>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF41" s="15"/>
+      <c r="AG41" s="11"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="11" t="s">
+      <c r="B42" s="14"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="11"/>
+      <c r="G42" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11" t="s">
+      <c r="I42" s="11"/>
+      <c r="J42" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="K42" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11" t="s">
+      <c r="L42" s="11"/>
+      <c r="M42" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="M42" s="11" t="s">
+      <c r="N42" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11" t="s">
+      <c r="O42" s="11"/>
+      <c r="P42" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="P42" s="11" t="s">
+      <c r="Q42" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11" t="s">
+      <c r="R42" s="11"/>
+      <c r="S42" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="S42" s="11" t="s">
+      <c r="T42" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11" t="s">
+      <c r="U42" s="11"/>
+      <c r="V42" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="V42" s="11" t="s">
+      <c r="W42" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="W42" s="11"/>
-      <c r="X42" s="11" t="s">
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="Y42" s="11" t="s">
+      <c r="Z42" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="Z42" s="11"/>
-      <c r="AA42" s="16" t="s">
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AB42" s="15" t="s">
+      <c r="AC42" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="AC42" s="15"/>
-      <c r="AD42" s="16" t="s">
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AE42" s="15" t="s">
+      <c r="AF42" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="AF42" s="11"/>
-    </row>
-    <row r="43" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG42" s="11"/>
+    </row>
+    <row r="43" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D43" s="10"/>
       <c r="E43" s="10"/>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G43" s="10"/>
       <c r="H43" s="10"/>
-      <c r="I43" s="10" t="s">
+      <c r="I43" s="10"/>
+      <c r="J43" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="J43" s="10"/>
       <c r="K43" s="10"/>
-      <c r="L43" s="10" t="s">
+      <c r="L43" s="10"/>
+      <c r="M43" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="M43" s="10"/>
       <c r="N43" s="10"/>
-      <c r="O43" s="10" t="s">
+      <c r="O43" s="10"/>
+      <c r="P43" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
-      <c r="R43" s="10" t="s">
+      <c r="R43" s="10"/>
+      <c r="S43" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="S43" s="10"/>
       <c r="T43" s="10"/>
-      <c r="U43" s="10" t="s">
+      <c r="U43" s="10"/>
+      <c r="V43" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="V43" s="10"/>
       <c r="W43" s="10"/>
-      <c r="X43" s="10" t="s">
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="Y43" s="10"/>
       <c r="Z43" s="10"/>
-      <c r="AA43" s="31" t="s">
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="AB43" s="32"/>
       <c r="AC43" s="32"/>
-      <c r="AD43" s="31" t="s">
+      <c r="AD43" s="32"/>
+      <c r="AE43" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="AE43" s="32"/>
-      <c r="AF43" s="10"/>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF43" s="32"/>
+      <c r="AG43" s="10"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="13"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="H44" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10" t="s">
+      <c r="I44" s="10"/>
+      <c r="J44" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="J44" s="10" t="s">
+      <c r="K44" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10" t="s">
+      <c r="L44" s="10"/>
+      <c r="M44" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="M44" s="10" t="s">
+      <c r="N44" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10" t="s">
+      <c r="O44" s="10"/>
+      <c r="P44" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="P44" s="10" t="s">
+      <c r="Q44" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10" t="s">
+      <c r="R44" s="10"/>
+      <c r="S44" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="S44" s="10" t="s">
+      <c r="T44" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10" t="s">
+      <c r="U44" s="10"/>
+      <c r="V44" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="V44" s="10" t="s">
+      <c r="W44" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="W44" s="10"/>
-      <c r="X44" s="10" t="s">
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="Y44" s="10" t="s">
+      <c r="Z44" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="Z44" s="10"/>
-      <c r="AA44" s="31" t="s">
+      <c r="AA44" s="10"/>
+      <c r="AB44" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AB44" s="32" t="s">
+      <c r="AC44" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="AC44" s="32"/>
-      <c r="AD44" s="31" t="s">
+      <c r="AD44" s="32"/>
+      <c r="AE44" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AE44" s="32" t="s">
+      <c r="AF44" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="AF44" s="10"/>
-    </row>
-    <row r="45" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG44" s="10"/>
+    </row>
+    <row r="45" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D45" s="11"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="11"/>
+      <c r="G45" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="G45" s="11"/>
       <c r="H45" s="11"/>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="11"/>
+      <c r="J45" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="J45" s="11"/>
       <c r="K45" s="11"/>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="11"/>
+      <c r="M45" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="M45" s="11"/>
       <c r="N45" s="11"/>
-      <c r="O45" s="11" t="s">
+      <c r="O45" s="11"/>
+      <c r="P45" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="P45" s="11"/>
       <c r="Q45" s="11"/>
-      <c r="R45" s="11" t="s">
+      <c r="R45" s="11"/>
+      <c r="S45" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="S45" s="11"/>
       <c r="T45" s="11"/>
-      <c r="U45" s="11" t="s">
+      <c r="U45" s="11"/>
+      <c r="V45" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="V45" s="11"/>
       <c r="W45" s="11"/>
-      <c r="X45" s="11" t="s">
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="Y45" s="11"/>
       <c r="Z45" s="11"/>
-      <c r="AA45" s="16" t="s">
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="AB45" s="15"/>
       <c r="AC45" s="15"/>
-      <c r="AD45" s="16" t="s">
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="AE45" s="15"/>
-      <c r="AF45" s="11"/>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="11"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="11" t="s">
+      <c r="B46" s="14"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="11"/>
+      <c r="G46" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="H46" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11" t="s">
+      <c r="I46" s="11"/>
+      <c r="J46" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="J46" s="11" t="s">
+      <c r="K46" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11" t="s">
+      <c r="L46" s="11"/>
+      <c r="M46" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="M46" s="11" t="s">
+      <c r="N46" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11" t="s">
+      <c r="O46" s="11"/>
+      <c r="P46" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="P46" s="11" t="s">
+      <c r="Q46" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11" t="s">
+      <c r="R46" s="11"/>
+      <c r="S46" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="S46" s="11" t="s">
+      <c r="T46" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="T46" s="11"/>
-      <c r="U46" s="11" t="s">
+      <c r="U46" s="11"/>
+      <c r="V46" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="V46" s="11" t="s">
+      <c r="W46" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="W46" s="11"/>
-      <c r="X46" s="11" t="s">
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="Y46" s="11" t="s">
+      <c r="Z46" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="Z46" s="11"/>
-      <c r="AA46" s="16" t="s">
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AB46" s="15" t="s">
+      <c r="AC46" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="16" t="s">
+      <c r="AD46" s="15"/>
+      <c r="AE46" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AE46" s="15" t="s">
+      <c r="AF46" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="AF46" s="11"/>
-    </row>
-    <row r="47" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+      <c r="AG46" s="11"/>
+    </row>
+    <row r="47" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="D47" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D47" s="10"/>
       <c r="E47" s="10"/>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="G47" s="10"/>
       <c r="H47" s="10"/>
-      <c r="I47" s="10" t="s">
+      <c r="I47" s="10"/>
+      <c r="J47" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="J47" s="10"/>
       <c r="K47" s="10"/>
-      <c r="L47" s="10" t="s">
+      <c r="L47" s="10"/>
+      <c r="M47" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="M47" s="10"/>
       <c r="N47" s="10"/>
-      <c r="O47" s="10" t="s">
+      <c r="O47" s="10"/>
+      <c r="P47" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="P47" s="10"/>
       <c r="Q47" s="10"/>
-      <c r="R47" s="10" t="s">
+      <c r="R47" s="10"/>
+      <c r="S47" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="S47" s="10"/>
       <c r="T47" s="10"/>
-      <c r="U47" s="10" t="s">
+      <c r="U47" s="10"/>
+      <c r="V47" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="V47" s="10"/>
       <c r="W47" s="10"/>
-      <c r="X47" s="10" t="s">
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="Y47" s="10"/>
       <c r="Z47" s="10"/>
-      <c r="AA47" s="31" t="s">
+      <c r="AA47" s="10"/>
+      <c r="AB47" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="AB47" s="32"/>
       <c r="AC47" s="32"/>
-      <c r="AD47" s="31" t="s">
+      <c r="AD47" s="32"/>
+      <c r="AE47" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="AE47" s="32"/>
-      <c r="AF47" s="10"/>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF47" s="32"/>
+      <c r="AG47" s="10"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="10" t="s">
+      <c r="B48" s="13"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="E48" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="H48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10" t="s">
+      <c r="I48" s="10"/>
+      <c r="J48" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="J48" s="10" t="s">
+      <c r="K48" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10" t="s">
+      <c r="L48" s="10"/>
+      <c r="M48" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="M48" s="10" t="s">
+      <c r="N48" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10" t="s">
+      <c r="O48" s="10"/>
+      <c r="P48" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="P48" s="10" t="s">
+      <c r="Q48" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10" t="s">
+      <c r="R48" s="10"/>
+      <c r="S48" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="S48" s="10" t="s">
+      <c r="T48" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="T48" s="10"/>
-      <c r="U48" s="10" t="s">
+      <c r="U48" s="10"/>
+      <c r="V48" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="V48" s="10" t="s">
+      <c r="W48" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="W48" s="10"/>
-      <c r="X48" s="10" t="s">
+      <c r="X48" s="10"/>
+      <c r="Y48" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="Y48" s="10" t="s">
+      <c r="Z48" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="Z48" s="10"/>
-      <c r="AA48" s="31" t="s">
+      <c r="AA48" s="10"/>
+      <c r="AB48" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AB48" s="32" t="s">
+      <c r="AC48" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="AC48" s="32"/>
-      <c r="AD48" s="31" t="s">
+      <c r="AD48" s="32"/>
+      <c r="AE48" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AE48" s="32" t="s">
+      <c r="AF48" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="AF48" s="10"/>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG48" s="10"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="E49" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11">
+      <c r="F49" s="11"/>
+      <c r="G49" s="11">
         <v>1</v>
       </c>
-      <c r="G49" s="11">
+      <c r="H49" s="11">
         <v>2</v>
       </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11">
+      <c r="I49" s="11"/>
+      <c r="J49" s="11">
         <v>0</v>
       </c>
-      <c r="J49" s="11">
+      <c r="K49" s="11">
         <v>1</v>
       </c>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11">
+      <c r="L49" s="11"/>
+      <c r="M49" s="11">
         <v>7777</v>
       </c>
-      <c r="M49" s="15" t="s">
+      <c r="N49" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="N49" s="11"/>
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
@@ -3735,11 +3884,12 @@
       <c r="AD49" s="11"/>
       <c r="AE49" s="11"/>
       <c r="AF49" s="11"/>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG49" s="11"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="6"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -3769,39 +3919,41 @@
       <c r="AD50" s="11"/>
       <c r="AE50" s="11"/>
       <c r="AF50" s="11"/>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG50" s="11"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="28"/>
+      <c r="C51" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="30">
+      <c r="D51" s="30">
         <v>7777</v>
       </c>
-      <c r="D51" s="30">
+      <c r="E51" s="30">
         <v>0</v>
       </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30">
+      <c r="F51" s="30"/>
+      <c r="G51" s="30">
         <v>1111</v>
       </c>
-      <c r="G51" s="30">
+      <c r="H51" s="30">
         <v>0</v>
       </c>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30">
-        <v>0</v>
-      </c>
+      <c r="I51" s="30"/>
       <c r="J51" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K51" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="8"/>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
@@ -3809,25 +3961,112 @@
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="10"/>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="5"/>
+      <c r="C55" s="2" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" s="36"/>
+      <c r="C57" s="37" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A59" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A60" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A61" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A62" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A63" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A64" s="36"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" s="36" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed RTR variable returns.  Tested and passed.
</commit_message>
<xml_diff>
--- a/Docs/Testing Plan.xlsx
+++ b/Docs/Testing Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="204">
   <si>
     <t>PDP-8 Instruction List</t>
   </si>
@@ -623,13 +623,16 @@
   </si>
   <si>
     <t>SWP</t>
+  </si>
+  <si>
+    <t>Testing Complete per KB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,6 +680,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -797,15 +808,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,6 +885,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,10 +1241,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="31"/>
       <c r="F1" t="s">
         <v>71</v>
       </c>
@@ -1304,20 +1318,22 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="2"/>
       <c r="D4">
         <v>7777</v>
       </c>
@@ -1338,2734 +1354,2738 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21"/>
     </row>
     <row r="12" spans="1:33" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="22"/>
+      <c r="G12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24" t="s">
+      <c r="I12" s="22"/>
+      <c r="J12" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="22"/>
+      <c r="M12" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24" t="s">
+      <c r="O12" s="22"/>
+      <c r="P12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="Q12" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24" t="s">
+      <c r="R12" s="22"/>
+      <c r="S12" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="T12" s="24" t="s">
+      <c r="T12" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24" t="s">
+      <c r="U12" s="22"/>
+      <c r="V12" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="W12" s="24" t="s">
+      <c r="W12" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24" t="s">
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Z12" s="24" t="s">
+      <c r="Z12" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24" t="s">
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AC12" s="24" t="s">
+      <c r="AC12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24" t="s">
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AF12" s="24" t="s">
+      <c r="AF12" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="AG12" s="24"/>
+      <c r="AG12" s="22"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="21" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21" t="s">
+      <c r="I13" s="19"/>
+      <c r="J13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21" t="s">
+      <c r="L13" s="19"/>
+      <c r="M13" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21" t="s">
+      <c r="O13" s="19"/>
+      <c r="P13" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21" t="s">
+      <c r="R13" s="19"/>
+      <c r="S13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="T13" s="21" t="s">
+      <c r="T13" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21" t="s">
+      <c r="U13" s="19"/>
+      <c r="V13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="W13" s="21" t="s">
+      <c r="W13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21" t="s">
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="Z13" s="21" t="s">
+      <c r="Z13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21" t="s">
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="AC13" s="21" t="s">
+      <c r="AC13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="21" t="s">
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="AF13" s="21" t="s">
+      <c r="AF13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="AG13" s="21"/>
+      <c r="AG13" s="19"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="8">
         <v>7777</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>0</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
         <v>1111</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="8">
         <v>0</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8">
         <v>0</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="8">
         <v>0</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
     </row>
     <row r="17" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9" t="s">
+      <c r="I17" s="7"/>
+      <c r="J17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9" t="s">
+      <c r="L17" s="7"/>
+      <c r="M17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9" t="s">
+      <c r="O17" s="7"/>
+      <c r="P17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="Q17" s="9" t="s">
+      <c r="Q17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9" t="s">
+      <c r="R17" s="7"/>
+      <c r="S17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="T17" s="9" t="s">
+      <c r="T17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9" t="s">
+      <c r="U17" s="7"/>
+      <c r="V17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="W17" s="9" t="s">
+      <c r="W17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9" t="s">
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="Z17" s="9" t="s">
+      <c r="Z17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AA17" s="9"/>
-      <c r="AB17" s="9" t="s">
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="AC17" s="9" t="s">
+      <c r="AC17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9" t="s">
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="AF17" s="9" t="s">
+      <c r="AF17" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AG17" s="9"/>
+      <c r="AG17" s="7"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="9" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9" t="s">
+      <c r="I18" s="7"/>
+      <c r="J18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9" t="s">
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="N18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9" t="s">
+      <c r="O18" s="7"/>
+      <c r="P18" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="Q18" s="9" t="s">
+      <c r="Q18" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9" t="s">
+      <c r="R18" s="7"/>
+      <c r="S18" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="T18" s="9" t="s">
+      <c r="T18" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9" t="s">
+      <c r="U18" s="7"/>
+      <c r="V18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="W18" s="9" t="s">
+      <c r="W18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9" t="s">
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Z18" s="9" t="s">
+      <c r="Z18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AA18" s="9"/>
-      <c r="AB18" s="9" t="s">
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AC18" s="9" t="s">
+      <c r="AC18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AD18" s="9"/>
-      <c r="AE18" s="9" t="s">
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AF18" s="9" t="s">
+      <c r="AF18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="AG18" s="9"/>
+      <c r="AG18" s="7"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10" t="s">
+      <c r="L19" s="8"/>
+      <c r="M19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10" t="s">
+      <c r="O19" s="8"/>
+      <c r="P19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Q19" s="10" t="s">
+      <c r="Q19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10" t="s">
+      <c r="R19" s="8"/>
+      <c r="S19" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="T19" s="10" t="s">
+      <c r="T19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
+      <c r="I23" s="8"/>
+      <c r="J23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10" t="s">
+      <c r="L23" s="8"/>
+      <c r="M23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10" t="s">
+      <c r="O23" s="8"/>
+      <c r="P23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="Q23" s="10" t="s">
+      <c r="Q23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10" t="s">
+      <c r="R23" s="8"/>
+      <c r="S23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="T23" s="10" t="s">
+      <c r="T23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10" t="s">
+      <c r="U23" s="8"/>
+      <c r="V23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="W23" s="10" t="s">
+      <c r="W23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10" t="s">
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z23" s="10" t="s">
+      <c r="Z23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10" t="s">
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AC23" s="10" t="s">
+      <c r="AC23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10" t="s">
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AF23" s="10" t="s">
+      <c r="AF23" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AG23" s="10"/>
+      <c r="AG23" s="8"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="10" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10" t="s">
+      <c r="I24" s="8"/>
+      <c r="J24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="K24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10" t="s">
+      <c r="L24" s="8"/>
+      <c r="M24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N24" s="10" t="s">
+      <c r="N24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10" t="s">
+      <c r="O24" s="8"/>
+      <c r="P24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q24" s="10" t="s">
+      <c r="Q24" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10" t="s">
+      <c r="R24" s="8"/>
+      <c r="S24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="T24" s="10" t="s">
+      <c r="T24" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10" t="s">
+      <c r="U24" s="8"/>
+      <c r="V24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="W24" s="10" t="s">
+      <c r="W24" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10" t="s">
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="Z24" s="10" t="s">
+      <c r="Z24" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AA24" s="10"/>
-      <c r="AB24" s="10" t="s">
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AC24" s="10" t="s">
+      <c r="AC24" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="10" t="s">
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AF24" s="10" t="s">
+      <c r="AF24" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AG24" s="10"/>
+      <c r="AG24" s="8"/>
     </row>
     <row r="25" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11" t="s">
+      <c r="I25" s="9"/>
+      <c r="J25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="K25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11" t="s">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11" t="s">
+      <c r="O25" s="9"/>
+      <c r="P25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="Q25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11" t="s">
+      <c r="R25" s="9"/>
+      <c r="S25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="T25" s="9" t="s">
+      <c r="T25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11" t="s">
+      <c r="U25" s="9"/>
+      <c r="V25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="W25" s="9" t="s">
+      <c r="W25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11" t="s">
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="Z25" s="9" t="s">
+      <c r="Z25" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="11" t="s">
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AC25" s="9" t="s">
+      <c r="AC25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AD25" s="11"/>
-      <c r="AE25" s="11" t="s">
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AF25" s="9" t="s">
+      <c r="AF25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AG25" s="11"/>
+      <c r="AG25" s="9"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="11" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11" t="s">
+      <c r="F26" s="9"/>
+      <c r="G26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11" t="s">
+      <c r="I26" s="9"/>
+      <c r="J26" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11" t="s">
+      <c r="L26" s="9"/>
+      <c r="M26" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N26" s="11" t="s">
+      <c r="N26" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11" t="s">
+      <c r="O26" s="9"/>
+      <c r="P26" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="Q26" s="11" t="s">
+      <c r="Q26" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11" t="s">
+      <c r="R26" s="9"/>
+      <c r="S26" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="T26" s="11" t="s">
+      <c r="T26" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11" t="s">
+      <c r="U26" s="9"/>
+      <c r="V26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="W26" s="11" t="s">
+      <c r="W26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11" t="s">
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="Z26" s="11" t="s">
+      <c r="Z26" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="11" t="s">
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AC26" s="11" t="s">
+      <c r="AC26" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="11" t="s">
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AF26" s="11" t="s">
+      <c r="AF26" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="AG26" s="11"/>
+      <c r="AG26" s="9"/>
     </row>
     <row r="27" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10" t="s">
+      <c r="I27" s="8"/>
+      <c r="J27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="K27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10" t="s">
+      <c r="L27" s="8"/>
+      <c r="M27" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10" t="s">
+      <c r="O27" s="8"/>
+      <c r="P27" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="Q27" s="10" t="s">
+      <c r="Q27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10" t="s">
+      <c r="R27" s="8"/>
+      <c r="S27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="T27" s="10" t="s">
+      <c r="T27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10" t="s">
+      <c r="U27" s="8"/>
+      <c r="V27" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="W27" s="10" t="s">
+      <c r="W27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10" t="s">
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z27" s="10" t="s">
+      <c r="Z27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AA27" s="10"/>
-      <c r="AB27" s="10" t="s">
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AC27" s="10" t="s">
+      <c r="AC27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AD27" s="10"/>
-      <c r="AE27" s="10" t="s">
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AF27" s="10" t="s">
+      <c r="AF27" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AG27" s="10"/>
+      <c r="AG27" s="8"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="10" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10" t="s">
+      <c r="I28" s="8"/>
+      <c r="J28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K28" s="10" t="s">
+      <c r="K28" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10" t="s">
+      <c r="L28" s="8"/>
+      <c r="M28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N28" s="10" t="s">
+      <c r="N28" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10" t="s">
+      <c r="O28" s="8"/>
+      <c r="P28" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q28" s="10" t="s">
+      <c r="Q28" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10" t="s">
+      <c r="R28" s="8"/>
+      <c r="S28" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="T28" s="10" t="s">
+      <c r="T28" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10" t="s">
+      <c r="U28" s="8"/>
+      <c r="V28" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="W28" s="10" t="s">
+      <c r="W28" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="X28" s="10"/>
-      <c r="Y28" s="10" t="s">
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Z28" s="10" t="s">
+      <c r="Z28" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AA28" s="10"/>
-      <c r="AB28" s="10" t="s">
+      <c r="AA28" s="8"/>
+      <c r="AB28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AC28" s="10" t="s">
+      <c r="AC28" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AD28" s="10"/>
-      <c r="AE28" s="10" t="s">
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AF28" s="10" t="s">
+      <c r="AF28" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="AG28" s="10"/>
+      <c r="AG28" s="8"/>
     </row>
     <row r="29" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11" t="s">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="9"/>
+      <c r="J29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11" t="s">
+      <c r="L29" s="9"/>
+      <c r="M29" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N29" s="9" t="s">
+      <c r="N29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11" t="s">
+      <c r="O29" s="9"/>
+      <c r="P29" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="Q29" s="9" t="s">
+      <c r="Q29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11" t="s">
+      <c r="R29" s="9"/>
+      <c r="S29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="T29" s="9" t="s">
+      <c r="T29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="U29" s="11"/>
-      <c r="V29" s="16" t="s">
+      <c r="U29" s="9"/>
+      <c r="V29" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="W29" s="9" t="s">
+      <c r="W29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="16" t="s">
+      <c r="X29" s="9"/>
+      <c r="Y29" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="Z29" s="9" t="s">
+      <c r="Z29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="16" t="s">
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AC29" s="9" t="s">
+      <c r="AC29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AD29" s="11"/>
-      <c r="AE29" s="15" t="s">
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="AF29" s="9" t="s">
+      <c r="AF29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AG29" s="11"/>
+      <c r="AG29" s="9"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="11" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11" t="s">
+      <c r="F30" s="9"/>
+      <c r="G30" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11" t="s">
+      <c r="I30" s="9"/>
+      <c r="J30" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K30" s="11" t="s">
+      <c r="K30" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11" t="s">
+      <c r="L30" s="9"/>
+      <c r="M30" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="N30" s="11" t="s">
+      <c r="N30" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11" t="s">
+      <c r="O30" s="9"/>
+      <c r="P30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="11" t="s">
+      <c r="Q30" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11" t="s">
+      <c r="R30" s="9"/>
+      <c r="S30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="T30" s="11" t="s">
+      <c r="T30" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11" t="s">
+      <c r="U30" s="9"/>
+      <c r="V30" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="W30" s="11" t="s">
+      <c r="W30" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11" t="s">
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="Z30" s="11" t="s">
+      <c r="Z30" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11" t="s">
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AC30" s="11" t="s">
+      <c r="AC30" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="AD30" s="11"/>
-      <c r="AE30" s="11" t="s">
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="AF30" s="11" t="s">
+      <c r="AF30" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AG30" s="11"/>
+      <c r="AG30" s="9"/>
     </row>
     <row r="31" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
+      <c r="F31" s="8"/>
+      <c r="G31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10" t="s">
+      <c r="I31" s="8"/>
+      <c r="J31" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="K31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10" t="s">
+      <c r="L31" s="8"/>
+      <c r="M31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="N31" s="10" t="s">
+      <c r="N31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10" t="s">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="Q31" s="10" t="s">
+      <c r="Q31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10" t="s">
+      <c r="R31" s="8"/>
+      <c r="S31" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="T31" s="10" t="s">
+      <c r="T31" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10" t="s">
+      <c r="U31" s="8"/>
+      <c r="V31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="W31" s="10" t="s">
+      <c r="W31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="X31" s="10"/>
-      <c r="Y31" s="10" t="s">
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Z31" s="10" t="s">
+      <c r="Z31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AA31" s="10"/>
-      <c r="AB31" s="10" t="s">
+      <c r="AA31" s="8"/>
+      <c r="AB31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AC31" s="10" t="s">
+      <c r="AC31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AD31" s="10"/>
-      <c r="AE31" s="10" t="s">
+      <c r="AD31" s="8"/>
+      <c r="AE31" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AF31" s="10" t="s">
+      <c r="AF31" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AG31" s="10"/>
+      <c r="AG31" s="8"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="F32" s="8"/>
+      <c r="G32" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10" t="s">
+      <c r="I32" s="8"/>
+      <c r="J32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K32" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10" t="s">
+      <c r="L32" s="8"/>
+      <c r="M32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N32" s="10" t="s">
+      <c r="N32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10" t="s">
+      <c r="O32" s="8"/>
+      <c r="P32" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="Q32" s="10" t="s">
+      <c r="Q32" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10" t="s">
+      <c r="R32" s="8"/>
+      <c r="S32" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="T32" s="10" t="s">
+      <c r="T32" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10" t="s">
+      <c r="U32" s="8"/>
+      <c r="V32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="W32" s="10" t="s">
+      <c r="W32" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="10" t="s">
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Z32" s="10" t="s">
+      <c r="Z32" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="AA32" s="10"/>
-      <c r="AB32" s="10" t="s">
+      <c r="AA32" s="8"/>
+      <c r="AB32" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AC32" s="10" t="s">
+      <c r="AC32" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="10" t="s">
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AF32" s="10" t="s">
+      <c r="AF32" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="AG32" s="10"/>
+      <c r="AG32" s="8"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="17"/>
-      <c r="X33" s="17"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="17"/>
-      <c r="AA33" s="17"/>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="17"/>
-      <c r="AF33" s="17"/>
-      <c r="AG33" s="17"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="15"/>
+      <c r="AE33" s="15"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17"/>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17"/>
-      <c r="AG34" s="17"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
     </row>
     <row r="35" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="26"/>
-      <c r="Y35" s="26"/>
-      <c r="Z35" s="26"/>
-      <c r="AA35" s="26"/>
-      <c r="AB35" s="26"/>
-      <c r="AC35" s="26"/>
-      <c r="AD35" s="26"/>
-      <c r="AE35" s="26"/>
-      <c r="AF35" s="26"/>
-      <c r="AG35" s="26"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="24"/>
+      <c r="V35" s="24"/>
+      <c r="W35" s="24"/>
+      <c r="X35" s="24"/>
+      <c r="Y35" s="24"/>
+      <c r="Z35" s="24"/>
+      <c r="AA35" s="24"/>
+      <c r="AB35" s="24"/>
+      <c r="AC35" s="24"/>
+      <c r="AD35" s="24"/>
+      <c r="AE35" s="24"/>
+      <c r="AF35" s="24"/>
+      <c r="AG35" s="24"/>
     </row>
     <row r="36" spans="1:33" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="24" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24" t="s">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H36" s="24" t="s">
+      <c r="H36" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24" t="s">
+      <c r="I36" s="22"/>
+      <c r="J36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K36" s="24" t="s">
+      <c r="K36" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24" t="s">
+      <c r="L36" s="22"/>
+      <c r="M36" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="N36" s="24" t="s">
+      <c r="N36" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24" t="s">
+      <c r="O36" s="22"/>
+      <c r="P36" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="Q36" s="24" t="s">
+      <c r="Q36" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24" t="s">
+      <c r="R36" s="22"/>
+      <c r="S36" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="T36" s="24" t="s">
+      <c r="T36" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="U36" s="24"/>
-      <c r="V36" s="24" t="s">
+      <c r="U36" s="22"/>
+      <c r="V36" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="W36" s="24" t="s">
+      <c r="W36" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="X36" s="24"/>
-      <c r="Y36" s="24" t="s">
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Z36" s="24" t="s">
+      <c r="Z36" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AA36" s="24"/>
-      <c r="AB36" s="24" t="s">
+      <c r="AA36" s="22"/>
+      <c r="AB36" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="AC36" s="24" t="s">
+      <c r="AC36" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AD36" s="24"/>
-      <c r="AE36" s="24" t="s">
+      <c r="AD36" s="22"/>
+      <c r="AE36" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AF36" s="24" t="s">
+      <c r="AF36" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="AG36" s="24"/>
+      <c r="AG36" s="22"/>
     </row>
     <row r="37" spans="1:33" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11" t="s">
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11" t="s">
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11" t="s">
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11" t="s">
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11" t="s">
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11" t="s">
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="W37" s="11"/>
-      <c r="X37" s="11"/>
-      <c r="Y37" s="11" t="s">
+      <c r="W37" s="9"/>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="16" t="s">
+      <c r="Z37" s="9"/>
+      <c r="AA37" s="9"/>
+      <c r="AB37" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="AC37" s="15"/>
-      <c r="AD37" s="15"/>
-      <c r="AE37" s="16" t="s">
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="AF37" s="15"/>
-      <c r="AG37" s="11"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="9"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="11" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11" t="s">
+      <c r="F38" s="9"/>
+      <c r="G38" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="H38" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11" t="s">
+      <c r="I38" s="9"/>
+      <c r="J38" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11" t="s">
+      <c r="L38" s="9"/>
+      <c r="M38" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="N38" s="11" t="s">
+      <c r="N38" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11" t="s">
+      <c r="O38" s="9"/>
+      <c r="P38" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="Q38" s="11" t="s">
+      <c r="Q38" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11" t="s">
+      <c r="R38" s="9"/>
+      <c r="S38" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="T38" s="11" t="s">
+      <c r="T38" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="U38" s="11"/>
-      <c r="V38" s="11" t="s">
+      <c r="U38" s="9"/>
+      <c r="V38" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="W38" s="11" t="s">
+      <c r="W38" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="X38" s="11"/>
-      <c r="Y38" s="11" t="s">
+      <c r="X38" s="9"/>
+      <c r="Y38" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="Z38" s="11" t="s">
+      <c r="Z38" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="AA38" s="11"/>
-      <c r="AB38" s="16" t="s">
+      <c r="AA38" s="9"/>
+      <c r="AB38" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AC38" s="15" t="s">
+      <c r="AC38" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="16" t="s">
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AF38" s="15" t="s">
+      <c r="AF38" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="AG38" s="11"/>
+      <c r="AG38" s="9"/>
     </row>
     <row r="39" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10" t="s">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10" t="s">
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10" t="s">
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10" t="s">
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10" t="s">
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10" t="s">
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="W39" s="10"/>
-      <c r="X39" s="10"/>
-      <c r="Y39" s="10" t="s">
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="Z39" s="10"/>
-      <c r="AA39" s="10"/>
-      <c r="AB39" s="31" t="s">
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="8"/>
+      <c r="AB39" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="AC39" s="32"/>
-      <c r="AD39" s="32"/>
-      <c r="AE39" s="31" t="s">
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="30"/>
+      <c r="AE39" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="AF39" s="32"/>
-      <c r="AG39" s="10"/>
+      <c r="AF39" s="30"/>
+      <c r="AG39" s="8"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="10" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10" t="s">
+      <c r="I40" s="8"/>
+      <c r="J40" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="K40" s="10" t="s">
+      <c r="K40" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10" t="s">
+      <c r="L40" s="8"/>
+      <c r="M40" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="N40" s="10" t="s">
+      <c r="N40" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10" t="s">
+      <c r="O40" s="8"/>
+      <c r="P40" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="Q40" s="10" t="s">
+      <c r="Q40" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10" t="s">
+      <c r="R40" s="8"/>
+      <c r="S40" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="T40" s="10" t="s">
+      <c r="T40" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10" t="s">
+      <c r="U40" s="8"/>
+      <c r="V40" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="W40" s="10" t="s">
+      <c r="W40" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="X40" s="10"/>
-      <c r="Y40" s="10" t="s">
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="Z40" s="10" t="s">
+      <c r="Z40" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="AA40" s="10"/>
-      <c r="AB40" s="31" t="s">
+      <c r="AA40" s="8"/>
+      <c r="AB40" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AC40" s="32" t="s">
+      <c r="AC40" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="AD40" s="32"/>
-      <c r="AE40" s="31" t="s">
+      <c r="AD40" s="30"/>
+      <c r="AE40" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AF40" s="32" t="s">
+      <c r="AF40" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="AG40" s="10"/>
+      <c r="AG40" s="8"/>
     </row>
     <row r="41" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11" t="s">
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11" t="s">
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11" t="s">
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11" t="s">
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11" t="s">
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
-      <c r="V41" s="11" t="s">
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="W41" s="11"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="11" t="s">
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="Z41" s="11"/>
-      <c r="AA41" s="11"/>
-      <c r="AB41" s="16" t="s">
+      <c r="Z41" s="9"/>
+      <c r="AA41" s="9"/>
+      <c r="AB41" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="16" t="s">
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="AF41" s="15"/>
-      <c r="AG41" s="11"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="9"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="11" t="s">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11" t="s">
+      <c r="F42" s="9"/>
+      <c r="G42" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11" t="s">
+      <c r="I42" s="9"/>
+      <c r="J42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="K42" s="11" t="s">
+      <c r="K42" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11" t="s">
+      <c r="L42" s="9"/>
+      <c r="M42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="N42" s="11" t="s">
+      <c r="N42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11" t="s">
+      <c r="O42" s="9"/>
+      <c r="P42" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="Q42" s="11" t="s">
+      <c r="Q42" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11" t="s">
+      <c r="R42" s="9"/>
+      <c r="S42" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="T42" s="11" t="s">
+      <c r="T42" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="U42" s="11"/>
-      <c r="V42" s="11" t="s">
+      <c r="U42" s="9"/>
+      <c r="V42" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="W42" s="11" t="s">
+      <c r="W42" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="X42" s="11"/>
-      <c r="Y42" s="11" t="s">
+      <c r="X42" s="9"/>
+      <c r="Y42" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="Z42" s="11" t="s">
+      <c r="Z42" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="AA42" s="11"/>
-      <c r="AB42" s="16" t="s">
+      <c r="AA42" s="9"/>
+      <c r="AB42" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AC42" s="15" t="s">
+      <c r="AC42" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="AD42" s="15"/>
-      <c r="AE42" s="16" t="s">
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AF42" s="15" t="s">
+      <c r="AF42" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="AG42" s="11"/>
+      <c r="AG42" s="9"/>
     </row>
     <row r="43" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10" t="s">
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10" t="s">
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10" t="s">
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10" t="s">
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10" t="s">
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10" t="s">
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="W43" s="10"/>
-      <c r="X43" s="10"/>
-      <c r="Y43" s="10" t="s">
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="Z43" s="10"/>
-      <c r="AA43" s="10"/>
-      <c r="AB43" s="31" t="s">
+      <c r="Z43" s="8"/>
+      <c r="AA43" s="8"/>
+      <c r="AB43" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="AC43" s="32"/>
-      <c r="AD43" s="32"/>
-      <c r="AE43" s="31" t="s">
+      <c r="AC43" s="30"/>
+      <c r="AD43" s="30"/>
+      <c r="AE43" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="AF43" s="32"/>
-      <c r="AG43" s="10"/>
+      <c r="AF43" s="30"/>
+      <c r="AG43" s="8"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="10" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10" t="s">
+      <c r="F44" s="8"/>
+      <c r="G44" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10" t="s">
+      <c r="I44" s="8"/>
+      <c r="J44" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="K44" s="10" t="s">
+      <c r="K44" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10" t="s">
+      <c r="L44" s="8"/>
+      <c r="M44" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="N44" s="10" t="s">
+      <c r="N44" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10" t="s">
+      <c r="O44" s="8"/>
+      <c r="P44" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="Q44" s="10" t="s">
+      <c r="Q44" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10" t="s">
+      <c r="R44" s="8"/>
+      <c r="S44" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="T44" s="10" t="s">
+      <c r="T44" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10" t="s">
+      <c r="U44" s="8"/>
+      <c r="V44" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="W44" s="10" t="s">
+      <c r="W44" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="X44" s="10"/>
-      <c r="Y44" s="10" t="s">
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="Z44" s="10" t="s">
+      <c r="Z44" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="AA44" s="10"/>
-      <c r="AB44" s="31" t="s">
+      <c r="AA44" s="8"/>
+      <c r="AB44" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AC44" s="32" t="s">
+      <c r="AC44" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="AD44" s="32"/>
-      <c r="AE44" s="31" t="s">
+      <c r="AD44" s="30"/>
+      <c r="AE44" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AF44" s="32" t="s">
+      <c r="AF44" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="AG44" s="10"/>
+      <c r="AG44" s="8"/>
     </row>
     <row r="45" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="12"/>
+      <c r="C45" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11" t="s">
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11" t="s">
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11" t="s">
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11" t="s">
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11" t="s">
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
-      <c r="V45" s="11" t="s">
+      <c r="T45" s="9"/>
+      <c r="U45" s="9"/>
+      <c r="V45" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="W45" s="11"/>
-      <c r="X45" s="11"/>
-      <c r="Y45" s="11" t="s">
+      <c r="W45" s="9"/>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Z45" s="11"/>
-      <c r="AA45" s="11"/>
-      <c r="AB45" s="16" t="s">
+      <c r="Z45" s="9"/>
+      <c r="AA45" s="9"/>
+      <c r="AB45" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="AC45" s="15"/>
-      <c r="AD45" s="15"/>
-      <c r="AE45" s="16" t="s">
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="AF45" s="15"/>
-      <c r="AG45" s="11"/>
+      <c r="AF45" s="13"/>
+      <c r="AG45" s="9"/>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="11" t="s">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11" t="s">
+      <c r="F46" s="9"/>
+      <c r="G46" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11" t="s">
+      <c r="I46" s="9"/>
+      <c r="J46" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="K46" s="11" t="s">
+      <c r="K46" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11" t="s">
+      <c r="L46" s="9"/>
+      <c r="M46" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="N46" s="11" t="s">
+      <c r="N46" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11" t="s">
+      <c r="O46" s="9"/>
+      <c r="P46" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="Q46" s="11" t="s">
+      <c r="Q46" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11" t="s">
+      <c r="R46" s="9"/>
+      <c r="S46" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="T46" s="11" t="s">
+      <c r="T46" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="U46" s="11"/>
-      <c r="V46" s="11" t="s">
+      <c r="U46" s="9"/>
+      <c r="V46" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="W46" s="11" t="s">
+      <c r="W46" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="X46" s="11"/>
-      <c r="Y46" s="11" t="s">
+      <c r="X46" s="9"/>
+      <c r="Y46" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="Z46" s="11" t="s">
+      <c r="Z46" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="AA46" s="11"/>
-      <c r="AB46" s="16" t="s">
+      <c r="AA46" s="9"/>
+      <c r="AB46" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AC46" s="15" t="s">
+      <c r="AC46" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="16" t="s">
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="AF46" s="15" t="s">
+      <c r="AF46" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="AG46" s="11"/>
+      <c r="AG46" s="9"/>
     </row>
     <row r="47" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10" t="s">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10" t="s">
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10" t="s">
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10" t="s">
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10" t="s">
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="T47" s="10"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="10" t="s">
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="W47" s="10"/>
-      <c r="X47" s="10"/>
-      <c r="Y47" s="10" t="s">
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="Z47" s="10"/>
-      <c r="AA47" s="10"/>
-      <c r="AB47" s="31" t="s">
+      <c r="Z47" s="8"/>
+      <c r="AA47" s="8"/>
+      <c r="AB47" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="AC47" s="32"/>
-      <c r="AD47" s="32"/>
-      <c r="AE47" s="31" t="s">
+      <c r="AC47" s="30"/>
+      <c r="AD47" s="30"/>
+      <c r="AE47" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="AF47" s="32"/>
-      <c r="AG47" s="10"/>
+      <c r="AF47" s="30"/>
+      <c r="AG47" s="8"/>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="10" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10" t="s">
+      <c r="F48" s="8"/>
+      <c r="G48" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H48" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10" t="s">
+      <c r="I48" s="8"/>
+      <c r="J48" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="K48" s="10" t="s">
+      <c r="K48" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10" t="s">
+      <c r="L48" s="8"/>
+      <c r="M48" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="N48" s="10" t="s">
+      <c r="N48" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10" t="s">
+      <c r="O48" s="8"/>
+      <c r="P48" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="Q48" s="10" t="s">
+      <c r="Q48" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="R48" s="10"/>
-      <c r="S48" s="10" t="s">
+      <c r="R48" s="8"/>
+      <c r="S48" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="T48" s="10" t="s">
+      <c r="T48" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="U48" s="10"/>
-      <c r="V48" s="10" t="s">
+      <c r="U48" s="8"/>
+      <c r="V48" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="W48" s="10" t="s">
+      <c r="W48" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="X48" s="10"/>
-      <c r="Y48" s="10" t="s">
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="Z48" s="10" t="s">
+      <c r="Z48" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="AA48" s="10"/>
-      <c r="AB48" s="31" t="s">
+      <c r="AA48" s="8"/>
+      <c r="AB48" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AC48" s="32" t="s">
+      <c r="AC48" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="AD48" s="32"/>
-      <c r="AE48" s="31" t="s">
+      <c r="AD48" s="30"/>
+      <c r="AE48" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="AF48" s="32" t="s">
+      <c r="AF48" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="AG48" s="10"/>
+      <c r="AG48" s="8"/>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11">
+      <c r="F49" s="9"/>
+      <c r="G49" s="9">
         <v>1</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="9">
         <v>2</v>
       </c>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11">
+      <c r="I49" s="9"/>
+      <c r="J49" s="9">
         <v>0</v>
       </c>
-      <c r="K49" s="11">
+      <c r="K49" s="9">
         <v>1</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11">
+      <c r="L49" s="9"/>
+      <c r="M49" s="9">
         <v>7777</v>
       </c>
-      <c r="N49" s="15" t="s">
+      <c r="N49" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-      <c r="X49" s="11"/>
-      <c r="Y49" s="11"/>
-      <c r="Z49" s="11"/>
-      <c r="AA49" s="11"/>
-      <c r="AB49" s="11"/>
-      <c r="AC49" s="11"/>
-      <c r="AD49" s="11"/>
-      <c r="AE49" s="11"/>
-      <c r="AF49" s="11"/>
-      <c r="AG49" s="11"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="9"/>
+      <c r="X49" s="9"/>
+      <c r="Y49" s="9"/>
+      <c r="Z49" s="9"/>
+      <c r="AA49" s="9"/>
+      <c r="AB49" s="9"/>
+      <c r="AC49" s="9"/>
+      <c r="AD49" s="9"/>
+      <c r="AE49" s="9"/>
+      <c r="AF49" s="9"/>
+      <c r="AG49" s="9"/>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
-      <c r="V50" s="11"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-      <c r="Y50" s="11"/>
-      <c r="Z50" s="11"/>
-      <c r="AA50" s="11"/>
-      <c r="AB50" s="11"/>
-      <c r="AC50" s="11"/>
-      <c r="AD50" s="11"/>
-      <c r="AE50" s="11"/>
-      <c r="AF50" s="11"/>
-      <c r="AG50" s="11"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="9"/>
+      <c r="Z50" s="9"/>
+      <c r="AA50" s="9"/>
+      <c r="AB50" s="9"/>
+      <c r="AC50" s="9"/>
+      <c r="AD50" s="9"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="9"/>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="29" t="s">
+      <c r="B51" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="30">
+      <c r="D51" s="28">
         <v>7777</v>
       </c>
-      <c r="E51" s="30">
+      <c r="E51" s="28">
         <v>0</v>
       </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30">
+      <c r="F51" s="28"/>
+      <c r="G51" s="28">
         <v>1111</v>
       </c>
-      <c r="H51" s="30">
+      <c r="H51" s="28">
         <v>0</v>
       </c>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30">
+      <c r="I51" s="28"/>
+      <c r="J51" s="28">
         <v>0</v>
       </c>
-      <c r="K51" s="30">
+      <c r="K51" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="2"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="2" t="s">
+      <c r="B55" s="3"/>
+      <c r="C55" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:33" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="37" t="s">
+      <c r="B57" s="34"/>
+      <c r="C57" s="35" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+      <c r="A59" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="36" t="s">
+      <c r="C59" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C60" s="36" t="s">
+      <c r="C60" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C61" s="36" t="s">
+      <c r="C61" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C62" s="36" t="s">
+      <c r="C62" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
+      <c r="A63" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="36" t="s">
+      <c r="B63" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="34" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A64" s="36"/>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="38" t="s">
+      <c r="A65" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="36" t="s">
+      <c r="C65" s="34" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated micro 3 CLA instr test unit to just increment.
</commit_message>
<xml_diff>
--- a/Docs/Testing Plan.xlsx
+++ b/Docs/Testing Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="209">
   <si>
     <t>PDP-8 Instruction List</t>
   </si>
@@ -631,7 +631,16 @@
     <t>1st round complete</t>
   </si>
   <si>
-    <t>2nd round</t>
+    <t>2nd round test with PC checks</t>
+  </si>
+  <si>
+    <t>3'5</t>
+  </si>
+  <si>
+    <t>3'4</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,8 +1344,12 @@
       <c r="A3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="B3" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>206</v>
+      </c>
       <c r="D3" s="39" t="s">
         <v>203</v>
       </c>
@@ -1348,7 +1361,9 @@
       <c r="B4" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4">
         <v>7777</v>
@@ -1376,7 +1391,9 @@
       <c r="B5" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>193</v>
       </c>
@@ -1388,7 +1405,9 @@
       <c r="B6" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>193</v>
       </c>
@@ -1400,7 +1419,9 @@
       <c r="B7" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>193</v>
       </c>
@@ -1412,7 +1433,9 @@
       <c r="B8" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>193</v>
       </c>
@@ -1424,7 +1447,9 @@
       <c r="B9" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>192</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>193</v>
       </c>
@@ -1558,7 +1583,9 @@
         <v>9</v>
       </c>
       <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33" t="s">
+        <v>192</v>
+      </c>
       <c r="D13" s="19" t="s">
         <v>36</v>
       </c>
@@ -1676,7 +1703,9 @@
       <c r="B15" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1766,7 +1795,9 @@
       <c r="B17" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>192</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>44</v>
       </c>
@@ -1924,7 +1955,9 @@
       <c r="B19" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D19" s="6" t="s">
         <v>76</v>
       </c>
@@ -2026,7 +2059,9 @@
       <c r="B21" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D21" s="4" t="s">
         <v>89</v>
       </c>
@@ -2112,7 +2147,9 @@
       <c r="B23" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D23" s="6" t="s">
         <v>96</v>
       </c>
@@ -2270,7 +2307,9 @@
       <c r="B25" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D25" s="4" t="s">
         <v>103</v>
       </c>
@@ -2428,7 +2467,9 @@
       <c r="B27" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D27" s="6" t="s">
         <v>104</v>
       </c>
@@ -2586,7 +2627,9 @@
       <c r="B29" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>105</v>
       </c>
@@ -2744,7 +2787,9 @@
       <c r="B31" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D31" s="6" t="s">
         <v>106</v>
       </c>
@@ -3090,7 +3135,9 @@
       <c r="B37" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D37" s="4" t="s">
         <v>191</v>
       </c>
@@ -3228,7 +3275,9 @@
       <c r="B39" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D39" s="6" t="s">
         <v>139</v>
       </c>
@@ -3366,7 +3415,9 @@
       <c r="B41" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D41" s="4" t="s">
         <v>188</v>
       </c>
@@ -3504,7 +3555,9 @@
       <c r="B43" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D43" s="6" t="s">
         <v>141</v>
       </c>
@@ -3642,7 +3695,9 @@
       <c r="B45" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D45" s="4" t="s">
         <v>140</v>
       </c>
@@ -3780,7 +3835,9 @@
       <c r="B47" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="D47" s="6" t="s">
         <v>142</v>
       </c>
@@ -3918,7 +3975,9 @@
       <c r="B49" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C49" s="12"/>
+      <c r="C49" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D49" s="4" t="s">
         <v>143</v>
       </c>
@@ -4012,7 +4071,9 @@
       <c r="B51" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="26" t="s">
+        <v>192</v>
+      </c>
       <c r="D51" s="27" t="s">
         <v>43</v>
       </c>
@@ -4100,7 +4161,9 @@
       <c r="B59" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="34"/>
+      <c r="C59" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D59" s="34" t="s">
         <v>194</v>
       </c>
@@ -4112,7 +4175,9 @@
       <c r="B60" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C60" s="34"/>
+      <c r="C60" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D60" s="34" t="s">
         <v>194</v>
       </c>
@@ -4124,7 +4189,9 @@
       <c r="B61" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C61" s="34"/>
+      <c r="C61" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D61" s="34" t="s">
         <v>194</v>
       </c>
@@ -4136,7 +4203,9 @@
       <c r="B62" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C62" s="34"/>
+      <c r="C62" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D62" s="34" t="s">
         <v>194</v>
       </c>
@@ -4148,7 +4217,9 @@
       <c r="B63" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="34"/>
+      <c r="C63" s="34" t="s">
+        <v>208</v>
+      </c>
       <c r="D63" s="34" t="s">
         <v>194</v>
       </c>
@@ -4166,7 +4237,9 @@
       <c r="B65" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="34"/>
+      <c r="C65" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D65" s="34" t="s">
         <v>194</v>
       </c>

</xml_diff>